<commit_message>
indicators selection to csv (so can track changes)
</commit_message>
<xml_diff>
--- a/data/db_variables.xlsx
+++ b/data/db_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizaandrade\Documents\GitHub\institutional-assessment-dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9224C27B-A086-4852-8D83-669EB9EBCB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FD13DA-4A32-43B0-B626-2DEB833BC42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="20550" windowHeight="11835" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
   </bookViews>
   <sheets>
     <sheet name="GBID" sheetId="1" r:id="rId1"/>
@@ -46556,11 +46556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C41AAE3-2996-429D-924B-4E57D391677C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D30"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46613,7 +46612,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -46647,7 +46646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -46681,7 +46680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>382</v>
       </c>
@@ -46712,7 +46711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -46746,7 +46745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>282</v>
       </c>
@@ -46780,7 +46779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -46811,7 +46810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -46842,7 +46841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -46873,7 +46872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -46904,7 +46903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>285</v>
       </c>
@@ -46938,7 +46937,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>279</v>
       </c>
@@ -46972,7 +46971,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>291</v>
       </c>
@@ -47006,7 +47005,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>288</v>
       </c>
@@ -47040,7 +47039,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -47074,7 +47073,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -47173,7 +47172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -47309,7 +47308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -47343,7 +47342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>333</v>
       </c>
@@ -47581,7 +47580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>139</v>
       </c>
@@ -47615,7 +47614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>370</v>
       </c>
@@ -47648,7 +47647,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -47679,7 +47678,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -47710,7 +47709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>386</v>
       </c>
@@ -47744,7 +47743,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -47775,7 +47774,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>198</v>
       </c>
@@ -47809,7 +47808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>275</v>
       </c>
@@ -47843,7 +47842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -47877,7 +47876,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -47908,7 +47907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -47942,7 +47941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -47976,7 +47975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>192</v>
       </c>
@@ -48010,7 +48009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>190</v>
       </c>
@@ -48044,7 +48043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -48078,7 +48077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>389</v>
       </c>
@@ -48112,7 +48111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -48146,7 +48145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -48177,7 +48176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -48208,7 +48207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -48239,7 +48238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -48273,7 +48272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -48307,7 +48306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>238</v>
       </c>
@@ -48341,7 +48340,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>380</v>
       </c>
@@ -48375,7 +48374,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>223</v>
       </c>
@@ -48409,7 +48408,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>208</v>
       </c>
@@ -48443,7 +48442,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>220</v>
       </c>
@@ -48477,7 +48476,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -48511,7 +48510,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>229</v>
       </c>
@@ -48545,7 +48544,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>211</v>
       </c>
@@ -48579,7 +48578,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>232</v>
       </c>
@@ -48613,7 +48612,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>226</v>
       </c>
@@ -48647,7 +48646,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>214</v>
       </c>
@@ -48681,7 +48680,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -48716,7 +48715,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -48747,7 +48746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>387</v>
       </c>
@@ -48778,7 +48777,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>299</v>
       </c>
@@ -48814,7 +48813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -48850,7 +48849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>305</v>
       </c>
@@ -48886,7 +48885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>302</v>
       </c>
@@ -48922,7 +48921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>308</v>
       </c>
@@ -48958,7 +48957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>311</v>
       </c>
@@ -48994,7 +48993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -49030,7 +49029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>297</v>
       </c>
@@ -49066,7 +49065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -49102,7 +49101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>101</v>
       </c>
@@ -49138,7 +49137,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>108</v>
       </c>
@@ -49174,7 +49173,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -49205,7 +49204,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -49236,7 +49235,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -49267,7 +49266,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>164</v>
       </c>
@@ -49298,7 +49297,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -49329,7 +49328,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>156</v>
       </c>
@@ -49360,7 +49359,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>383</v>
       </c>
@@ -49391,7 +49390,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>150</v>
       </c>
@@ -49422,7 +49421,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -49453,7 +49452,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>201</v>
       </c>
@@ -49487,7 +49486,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>330</v>
       </c>
@@ -49521,7 +49520,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -49555,7 +49554,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>183</v>
       </c>
@@ -49586,7 +49585,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>245</v>
       </c>
@@ -49622,7 +49621,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>242</v>
       </c>
@@ -49658,7 +49657,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -49689,7 +49688,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -49720,7 +49719,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>173</v>
       </c>
@@ -49751,7 +49750,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>129</v>
       </c>
@@ -49782,7 +49781,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>350</v>
       </c>
@@ -49816,7 +49815,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>339</v>
       </c>
@@ -49850,7 +49849,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>119</v>
       </c>
@@ -49884,7 +49883,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>336</v>
       </c>
@@ -49918,7 +49917,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>347</v>
       </c>
@@ -49952,7 +49951,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>384</v>
       </c>
@@ -49986,7 +49985,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>342</v>
       </c>
@@ -50020,7 +50019,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>272</v>
       </c>
@@ -50054,7 +50053,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>269</v>
       </c>
@@ -50088,7 +50087,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>266</v>
       </c>
@@ -50122,7 +50121,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>263</v>
       </c>
@@ -50156,7 +50155,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>385</v>
       </c>
@@ -50190,7 +50189,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>381</v>
       </c>
@@ -50220,26 +50219,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K109" xr:uid="{D3B893D9-65E7-41EF-B122-17457A36849E}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Burden of government regulation, 1-7 (best)"/>
-        <filter val="Effectiveness of anti-monopoly policy, 1-7 (best)"/>
-        <filter val="Efficiency of legal framework in challenging regs., 1-7 (best)"/>
-        <filter val="Efficiency of legal framework in settling disputes, 1-7 (best)"/>
-        <filter val="Favoritism in decisions of government officials, 1-7 (best)"/>
-        <filter val="Hiring and firing practices, 1-7 (best)"/>
-        <filter val="Irregular payments and bribes, 1-7 (best)"/>
-        <filter val="Judicial independence, 1-7 (best)"/>
-        <filter val="Protection of minority shareholders interests, 1-7 (best)"/>
-        <filter val="Public trust in politicians, 1-7 (best)"/>
-        <filter val="Transparency of government policymaking, 1-7 (best)"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="World Economic Forum Global Competitiveness Index"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K109">
       <sortCondition descending="1" ref="K1:K109"/>
     </sortState>

</xml_diff>

<commit_message>
Fixed Diversion of public funds
</commit_message>
<xml_diff>
--- a/data/db_variables.xlsx
+++ b/data/db_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizaandrade\Documents\GitHub\institutional-assessment-dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kannanvenkat/Documents/worldBank/CLAIR/Dashboard/institutional-assessment-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FD13DA-4A32-43B0-B626-2DEB833BC42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F30D38-D46E-0C4F-ADA5-9E05174D3120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="20550" windowHeight="11835" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="20560" windowHeight="11840" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
   </bookViews>
   <sheets>
     <sheet name="GBID" sheetId="1" r:id="rId1"/>
@@ -46559,25 +46559,25 @@
   <dimension ref="A1:K109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="56.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="52.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="9" max="9" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.1640625" customWidth="1"/>
+    <col min="11" max="11" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>357</v>
       </c>
@@ -46612,7 +46612,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -46646,7 +46646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>132</v>
       </c>
@@ -46680,7 +46680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>382</v>
       </c>
@@ -46711,7 +46711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -46745,7 +46745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>282</v>
       </c>
@@ -46779,7 +46779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -46810,7 +46810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -46841,7 +46841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -46872,7 +46872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -46903,7 +46903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>285</v>
       </c>
@@ -46937,7 +46937,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>279</v>
       </c>
@@ -46971,7 +46971,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>291</v>
       </c>
@@ -47005,7 +47005,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>288</v>
       </c>
@@ -47039,7 +47039,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -47073,7 +47073,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -47104,7 +47104,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -47138,7 +47138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>294</v>
       </c>
@@ -47172,7 +47172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -47206,7 +47206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>254</v>
       </c>
@@ -47240,7 +47240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>251</v>
       </c>
@@ -47274,7 +47274,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>326</v>
       </c>
@@ -47308,7 +47308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -47342,7 +47342,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>333</v>
       </c>
@@ -47376,7 +47376,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>323</v>
       </c>
@@ -47410,7 +47410,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>320</v>
       </c>
@@ -47444,7 +47444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -47478,7 +47478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>248</v>
       </c>
@@ -47512,7 +47512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -47546,7 +47546,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -47580,7 +47580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>139</v>
       </c>
@@ -47614,7 +47614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>370</v>
       </c>
@@ -47647,7 +47647,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -47678,7 +47678,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -47709,7 +47709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>386</v>
       </c>
@@ -47743,7 +47743,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>105</v>
       </c>
@@ -47774,7 +47774,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>198</v>
       </c>
@@ -47808,7 +47808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>275</v>
       </c>
@@ -47842,7 +47842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>195</v>
       </c>
@@ -47876,7 +47876,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -47907,7 +47907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -47941,7 +47941,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>32</v>
       </c>
@@ -47975,7 +47975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>192</v>
       </c>
@@ -48009,7 +48009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>190</v>
       </c>
@@ -48043,7 +48043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -48077,7 +48077,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>389</v>
       </c>
@@ -48111,7 +48111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -48145,7 +48145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -48176,7 +48176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -48207,7 +48207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
@@ -48238,7 +48238,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>64</v>
       </c>
@@ -48272,7 +48272,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -48306,7 +48306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>238</v>
       </c>
@@ -48340,7 +48340,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>380</v>
       </c>
@@ -48374,7 +48374,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>223</v>
       </c>
@@ -48408,7 +48408,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>208</v>
       </c>
@@ -48442,7 +48442,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>220</v>
       </c>
@@ -48476,7 +48476,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -48510,7 +48510,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>229</v>
       </c>
@@ -48544,7 +48544,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>211</v>
       </c>
@@ -48578,7 +48578,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>232</v>
       </c>
@@ -48612,7 +48612,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>226</v>
       </c>
@@ -48646,7 +48646,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>214</v>
       </c>
@@ -48680,7 +48680,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>71</v>
       </c>
@@ -48715,7 +48715,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -48746,7 +48746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>387</v>
       </c>
@@ -48777,7 +48777,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>299</v>
       </c>
@@ -48813,7 +48813,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>40</v>
       </c>
@@ -48849,7 +48849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>305</v>
       </c>
@@ -48885,7 +48885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>302</v>
       </c>
@@ -48921,7 +48921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>308</v>
       </c>
@@ -48957,7 +48957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>311</v>
       </c>
@@ -48993,7 +48993,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>114</v>
       </c>
@@ -49029,7 +49029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>297</v>
       </c>
@@ -49065,7 +49065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -49101,7 +49101,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>101</v>
       </c>
@@ -49137,7 +49137,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>108</v>
       </c>
@@ -49173,7 +49173,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>187</v>
       </c>
@@ -49204,7 +49204,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -49235,7 +49235,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -49266,7 +49266,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>164</v>
       </c>
@@ -49297,7 +49297,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -49328,7 +49328,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>156</v>
       </c>
@@ -49359,7 +49359,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>383</v>
       </c>
@@ -49390,7 +49390,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>150</v>
       </c>
@@ -49421,7 +49421,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>144</v>
       </c>
@@ -49452,7 +49452,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>201</v>
       </c>
@@ -49486,12 +49486,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>330</v>
       </c>
       <c r="B88" s="3">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C88" t="str">
         <f>VLOOKUP(B88,'[1]Master - API'!$F:$G,2,0)</f>
@@ -49520,7 +49520,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>388</v>
       </c>
@@ -49554,7 +49554,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>183</v>
       </c>
@@ -49585,7 +49585,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>245</v>
       </c>
@@ -49621,7 +49621,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>242</v>
       </c>
@@ -49657,7 +49657,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -49688,7 +49688,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -49719,7 +49719,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>173</v>
       </c>
@@ -49750,7 +49750,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>129</v>
       </c>
@@ -49781,7 +49781,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>350</v>
       </c>
@@ -49815,7 +49815,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>339</v>
       </c>
@@ -49849,7 +49849,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>119</v>
       </c>
@@ -49883,7 +49883,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>336</v>
       </c>
@@ -49917,7 +49917,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>347</v>
       </c>
@@ -49951,7 +49951,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>384</v>
       </c>
@@ -49985,7 +49985,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>342</v>
       </c>
@@ -50019,7 +50019,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>272</v>
       </c>
@@ -50053,7 +50053,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>269</v>
       </c>
@@ -50087,7 +50087,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>266</v>
       </c>
@@ -50121,7 +50121,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>263</v>
       </c>
@@ -50155,7 +50155,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>385</v>
       </c>
@@ -50189,7 +50189,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>381</v>
       </c>
@@ -50218,11 +50218,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K109" xr:uid="{D3B893D9-65E7-41EF-B122-17457A36849E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K109">
-      <sortCondition descending="1" ref="K1:K109"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Sanitization of Code - Removed Global Corruption,Foreign Currency
</commit_message>
<xml_diff>
--- a/data/db_variables.xlsx
+++ b/data/db_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kannanvenkat/Documents/worldBank/CLAIR/Dashboard/institutional-assessment-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F30D38-D46E-0C4F-ADA5-9E05174D3120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A2C7AF-537F-144F-9897-6F9BC88C5CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="20560" windowHeight="11840" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GBID!$A$1:$K$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GBID!$A$1:$K$107</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="387">
   <si>
     <t>World Justice Project, Rule of Law</t>
   </si>
@@ -811,15 +811,6 @@
     <t>legaleff_challenging</t>
   </si>
   <si>
-    <t>Global Corruption Barometer</t>
-  </si>
-  <si>
-    <t>Transparency International's Global Corruption Barometer (TIGBC) is the largest world-wide public opinion survey on corruption. It addresses people's direct experiences with bribery and details their views on corruption in the main institutions in their countries. Significantly, the Barometer also provides insights into how willing and ready people are to act to stop corruption.</t>
-  </si>
-  <si>
-    <t>gcb_corruption</t>
-  </si>
-  <si>
     <t>Bertelsmann Transformation Index</t>
   </si>
   <si>
@@ -986,15 +977,6 @@
   </si>
   <si>
     <t>scopeofstateownedenterprises</t>
-  </si>
-  <si>
-    <t>WEF GCI Most Problematic Factors</t>
-  </si>
-  <si>
-    <t>Extent to which regulations over foreign currency is one of the most pressing obstacles for business</t>
-  </si>
-  <si>
-    <t>fx_constraint</t>
   </si>
   <si>
     <t>It measures business executives perceptions of their countrys efficiency of customs procedures.</t>
@@ -1207,13 +1189,7 @@
     <t>Steering capability</t>
   </si>
   <si>
-    <t>Foreign currency regulations</t>
-  </si>
-  <si>
     <t>Centre of government, influence</t>
-  </si>
-  <si>
-    <t>Global corruption barometer</t>
   </si>
   <si>
     <t>Impartial public administration</t>
@@ -46556,10 +46532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C41AAE3-2996-429D-924B-4E57D391677C}">
-  <dimension ref="A1:K109"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -46579,37 +46555,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -46633,7 +46609,7 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
@@ -46667,7 +46643,7 @@
         <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>17</v>
@@ -46682,7 +46658,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" t="s">
@@ -46698,7 +46674,7 @@
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>2</v>
@@ -46732,7 +46708,7 @@
         <v>118</v>
       </c>
       <c r="G5" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -46747,7 +46723,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B6" s="3">
         <v>27900</v>
@@ -46757,7 +46733,7 @@
         <v>Freedom of opinion and expression is effectively guaranteed</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
@@ -46766,14 +46742,14 @@
         <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="K6" t="s">
         <v>0</v>
@@ -46797,7 +46773,7 @@
         <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>2</v>
@@ -46828,7 +46804,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>2</v>
@@ -46859,7 +46835,7 @@
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>2</v>
@@ -46890,7 +46866,7 @@
         <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>2</v>
@@ -46905,7 +46881,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B11" s="3">
         <v>27894</v>
@@ -46915,7 +46891,7 @@
         <v>Complaint mechanisms</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>5</v>
@@ -46924,22 +46900,22 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="K11" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B12" s="3">
         <v>27904</v>
@@ -46949,7 +46925,7 @@
         <v>Fundamental labor rights are effectively guaranteed</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>5</v>
@@ -46958,22 +46934,22 @@
         <v>143</v>
       </c>
       <c r="G12" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="K12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B13" s="3">
         <v>27885</v>
@@ -46983,7 +46959,7 @@
         <v>Publicized laws and government data</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
@@ -46992,22 +46968,22 @@
         <v>3</v>
       </c>
       <c r="G13" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="K13" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B14" s="3">
         <v>27889</v>
@@ -47017,7 +46993,7 @@
         <v>Right to information</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>5</v>
@@ -47026,17 +47002,17 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="K14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -47060,7 +47036,7 @@
         <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>17</v>
@@ -47091,7 +47067,7 @@
         <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>2</v>
@@ -47125,7 +47101,7 @@
         <v>143</v>
       </c>
       <c r="G17" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>17</v>
@@ -47140,7 +47116,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B18" s="3">
         <v>40828</v>
@@ -47150,7 +47126,7 @@
         <v>Judicial independence, 1-7 (best)</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
@@ -47159,14 +47135,14 @@
         <v>118</v>
       </c>
       <c r="G18" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="K18" t="s">
         <v>15</v>
@@ -47193,7 +47169,7 @@
         <v>143</v>
       </c>
       <c r="G19" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>17</v>
@@ -47227,7 +47203,7 @@
         <v>118</v>
       </c>
       <c r="G20" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>17</v>
@@ -47261,7 +47237,7 @@
         <v>118</v>
       </c>
       <c r="G21" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>17</v>
@@ -47276,7 +47252,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="B22" s="3">
         <v>40818</v>
@@ -47286,7 +47262,7 @@
         <v>Irregular payments and bribes, 1-7 (best)</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>5</v>
@@ -47295,14 +47271,14 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I22" s="1"/>
       <c r="J22" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="K22" t="s">
         <v>15</v>
@@ -47329,7 +47305,7 @@
         <v>44</v>
       </c>
       <c r="G23" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>17</v>
@@ -47344,7 +47320,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B24" s="3">
         <v>41411</v>
@@ -47354,7 +47330,7 @@
         <v>GCI 4.0: Extent of market dominance</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>5</v>
@@ -47363,14 +47339,14 @@
         <v>89</v>
       </c>
       <c r="G24" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="K24" t="s">
         <v>15</v>
@@ -47378,7 +47354,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="B25" s="3">
         <v>40873</v>
@@ -47388,7 +47364,7 @@
         <v>Transparency of government policymaking, 1-7 (best)</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>5</v>
@@ -47397,14 +47373,14 @@
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="K25" t="s">
         <v>15</v>
@@ -47412,7 +47388,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="B26" s="3">
         <v>40947</v>
@@ -47422,7 +47398,7 @@
         <v>Effectiveness of anti-monopoly policy, 1-7 (best)</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>5</v>
@@ -47431,14 +47407,14 @@
         <v>89</v>
       </c>
       <c r="G26" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I26" s="1"/>
       <c r="J26" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K26" t="s">
         <v>15</v>
@@ -47465,7 +47441,7 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>17</v>
@@ -47499,7 +47475,7 @@
         <v>89</v>
       </c>
       <c r="G28" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>17</v>
@@ -47514,7 +47490,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B29" s="3">
         <v>41008</v>
@@ -47524,7 +47500,7 @@
         <v>Burden of government regulation, 1-7 (best)</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>5</v>
@@ -47533,14 +47509,14 @@
         <v>89</v>
       </c>
       <c r="G29" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="K29" t="s">
         <v>15</v>
@@ -47567,7 +47543,7 @@
         <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>17</v>
@@ -47601,7 +47577,7 @@
         <v>44</v>
       </c>
       <c r="G31" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>17</v>
@@ -47616,35 +47592,35 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B32">
         <v>946</v>
       </c>
       <c r="C32" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D32" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="G32" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="K32" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -47665,7 +47641,7 @@
         <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>2</v>
@@ -47696,10 +47672,10 @@
         <v>3</v>
       </c>
       <c r="G34" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" t="s">
@@ -47711,98 +47687,98 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>386</v>
-      </c>
-      <c r="B35" s="3">
-        <v>3285</v>
-      </c>
-      <c r="C35" t="str">
-        <f>VLOOKUP(B35,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Foreign Currency Regulations</v>
+        <v>105</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" t="s">
+        <v>105</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>315</v>
+        <v>106</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>163</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>376</v>
+        <v>89</v>
+      </c>
+      <c r="G35" t="s">
+        <v>366</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I35" s="1"/>
       <c r="J35" t="s">
-        <v>314</v>
+        <v>104</v>
       </c>
       <c r="K35" t="s">
-        <v>313</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" t="s">
-        <v>105</v>
+        <v>198</v>
+      </c>
+      <c r="B36" s="3">
+        <v>41825</v>
+      </c>
+      <c r="C36" t="str">
+        <f>VLOOKUP(B36,'[1]Master - API'!$F:$G,2,0)</f>
+        <v xml:space="preserve">Checks on government </v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="G36" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" t="s">
-        <v>104</v>
+        <v>197</v>
       </c>
       <c r="K36" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>272</v>
       </c>
       <c r="B37" s="3">
-        <v>41825</v>
+        <v>28738</v>
       </c>
       <c r="C37" t="str">
         <f>VLOOKUP(B37,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Checks on government </v>
+        <v>Civil society participation</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>199</v>
+        <v>273</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F37" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="G37" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I37" s="1"/>
-      <c r="J37" t="s">
-        <v>197</v>
+      <c r="J37" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="K37" t="s">
         <v>27</v>
@@ -47810,33 +47786,33 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>275</v>
+        <v>195</v>
       </c>
       <c r="B38" s="3">
-        <v>28738</v>
+        <v>41854</v>
       </c>
       <c r="C38" t="str">
         <f>VLOOKUP(B38,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Civil society participation</v>
+        <v xml:space="preserve">Corruption </v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>276</v>
+        <v>196</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F38" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="G38" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I38" s="1"/>
-      <c r="J38" s="4" t="s">
-        <v>274</v>
+      <c r="J38" t="s">
+        <v>194</v>
       </c>
       <c r="K38" t="s">
         <v>27</v>
@@ -47844,33 +47820,30 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>195</v>
-      </c>
-      <c r="B39" s="3">
-        <v>41854</v>
-      </c>
-      <c r="C39" t="str">
-        <f>VLOOKUP(B39,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Corruption </v>
+        <v>53</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" t="s">
+        <v>53</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>196</v>
+        <v>54</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" t="s">
-        <v>194</v>
+        <v>52</v>
       </c>
       <c r="K39" t="s">
         <v>27</v>
@@ -47878,30 +47851,33 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" t="s">
-        <v>53</v>
+        <v>35</v>
+      </c>
+      <c r="B40">
+        <v>41857</v>
+      </c>
+      <c r="C40" t="str">
+        <f>VLOOKUP(B40,'[1]Master - API'!$F:$G,2,0)</f>
+        <v xml:space="preserve">CSO entry and exit </v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="G40" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="K40" t="s">
         <v>27</v>
@@ -47909,17 +47885,17 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B41">
-        <v>41857</v>
+        <v>41881</v>
       </c>
       <c r="C41" t="str">
         <f>VLOOKUP(B41,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">CSO entry and exit </v>
+        <v xml:space="preserve">Engaged society </v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>5</v>
@@ -47928,14 +47904,14 @@
         <v>24</v>
       </c>
       <c r="G41" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I41" s="1"/>
       <c r="J41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K41" t="s">
         <v>27</v>
@@ -47943,26 +47919,26 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42">
-        <v>41881</v>
+        <v>192</v>
+      </c>
+      <c r="B42" s="3">
+        <v>41882</v>
       </c>
       <c r="C42" t="str">
         <f>VLOOKUP(B42,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Engaged society </v>
+        <v xml:space="preserve">Executive bribery and corrupt exchanges </v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>33</v>
+        <v>193</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="G42" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>17</v>
@@ -47977,33 +47953,33 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B43" s="3">
-        <v>41882</v>
+        <v>41883</v>
       </c>
       <c r="C43" t="str">
         <f>VLOOKUP(B43,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Executive bribery and corrupt exchanges </v>
+        <v xml:space="preserve">Executive constraints </v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F43" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="G43" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" t="s">
-        <v>31</v>
+        <v>189</v>
       </c>
       <c r="K43" t="s">
         <v>27</v>
@@ -48011,33 +47987,33 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>190</v>
-      </c>
-      <c r="B44" s="3">
-        <v>41883</v>
+        <v>29</v>
+      </c>
+      <c r="B44">
+        <v>41918</v>
       </c>
       <c r="C44" t="str">
         <f>VLOOKUP(B44,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Executive constraints </v>
+        <v xml:space="preserve">Freedom of academic and cultural expression </v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>191</v>
+        <v>30</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="G44" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" t="s">
-        <v>189</v>
+        <v>28</v>
       </c>
       <c r="K44" t="s">
         <v>27</v>
@@ -48045,33 +48021,33 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>381</v>
       </c>
       <c r="B45">
-        <v>41918</v>
+        <v>42084</v>
       </c>
       <c r="C45" t="str">
         <f>VLOOKUP(B45,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Freedom of academic and cultural expression </v>
+        <v xml:space="preserve">Rigorous and impartial public administration </v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F45" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I45" s="1"/>
       <c r="J45" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="K45" t="s">
         <v>27</v>
@@ -48079,33 +48055,33 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>389</v>
+        <v>122</v>
       </c>
       <c r="B46">
-        <v>42084</v>
+        <v>41951</v>
       </c>
       <c r="C46" t="str">
         <f>VLOOKUP(B46,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Rigorous and impartial public administration </v>
+        <v xml:space="preserve">Judicial accountability </v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F46" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="G46" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I46" s="1"/>
       <c r="J46" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="K46" t="s">
         <v>27</v>
@@ -48113,33 +48089,30 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>122</v>
-      </c>
-      <c r="B47">
-        <v>41951</v>
-      </c>
-      <c r="C47" t="str">
-        <f>VLOOKUP(B47,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Judicial accountability </v>
+        <v>80</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" t="s">
+        <v>80</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="G47" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="K47" t="s">
         <v>27</v>
@@ -48147,14 +48120,14 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>5</v>
@@ -48163,14 +48136,14 @@
         <v>60</v>
       </c>
       <c r="G48" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K48" t="s">
         <v>27</v>
@@ -48178,14 +48151,14 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>5</v>
@@ -48194,14 +48167,14 @@
         <v>60</v>
       </c>
       <c r="G49" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="K49" t="s">
         <v>27</v>
@@ -48209,14 +48182,17 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="B50">
+        <v>42025</v>
+      </c>
+      <c r="C50" t="str">
+        <f>VLOOKUP(B50,'[1]Master - API'!$F:$G,2,0)</f>
+        <v xml:space="preserve">Power distributed by social group </v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>5</v>
@@ -48225,14 +48201,14 @@
         <v>60</v>
       </c>
       <c r="G50" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I50" s="1"/>
       <c r="J50" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K50" t="s">
         <v>27</v>
@@ -48240,17 +48216,17 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B51">
-        <v>42025</v>
+        <v>42026</v>
       </c>
       <c r="C51" t="str">
         <f>VLOOKUP(B51,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Power distributed by social group </v>
+        <v xml:space="preserve">Power distributed by socio-economic position </v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>5</v>
@@ -48259,14 +48235,14 @@
         <v>60</v>
       </c>
       <c r="G51" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I51" s="1"/>
       <c r="J51" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K51" t="s">
         <v>27</v>
@@ -48274,17 +48250,17 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52">
-        <v>42026</v>
+        <v>238</v>
+      </c>
+      <c r="B52" s="3">
+        <v>40991</v>
       </c>
       <c r="C52" t="str">
         <f>VLOOKUP(B52,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Power distributed by socio-economic position </v>
+        <v>Party Financing</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>62</v>
+        <v>239</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>5</v>
@@ -48293,82 +48269,82 @@
         <v>60</v>
       </c>
       <c r="G52" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I52" s="1"/>
       <c r="J52" t="s">
-        <v>59</v>
+        <v>237</v>
       </c>
       <c r="K52" t="s">
-        <v>27</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>238</v>
+        <v>374</v>
       </c>
       <c r="B53" s="3">
-        <v>40991</v>
+        <v>41114</v>
       </c>
       <c r="C53" t="str">
         <f>VLOOKUP(B53,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Party Financing</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>239</v>
+        <v>Budget Documentation</v>
+      </c>
+      <c r="D53" t="s">
+        <v>235</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F53" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="G53" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K53" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>380</v>
+        <v>223</v>
       </c>
       <c r="B54" s="3">
-        <v>41114</v>
+        <v>41141</v>
       </c>
       <c r="C54" t="str">
         <f>VLOOKUP(B54,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Budget Documentation</v>
-      </c>
-      <c r="D54" t="s">
-        <v>235</v>
+        <v>Debt management</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G54" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I54" s="1"/>
       <c r="J54" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="K54" t="s">
         <v>206</v>
@@ -48376,33 +48352,33 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B55" s="3">
-        <v>41141</v>
+        <v>41216</v>
       </c>
       <c r="C55" t="str">
         <f>VLOOKUP(B55,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Debt management</v>
+        <v>External audit</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I55" s="1"/>
       <c r="J55" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="K55" t="s">
         <v>206</v>
@@ -48410,33 +48386,33 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="B56" s="3">
-        <v>41216</v>
+        <v>41149</v>
       </c>
       <c r="C56" t="str">
         <f>VLOOKUP(B56,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>External audit</v>
+        <v>Fiscal strategy</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G56" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I56" s="1"/>
       <c r="J56" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="K56" t="s">
         <v>206</v>
@@ -48444,33 +48420,33 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B57" s="3">
-        <v>41149</v>
+        <v>41162</v>
       </c>
       <c r="C57" t="str">
         <f>VLOOKUP(B57,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Fiscal strategy</v>
+        <v>Legislative scrutiny of budgets</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G57" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I57" s="1"/>
       <c r="J57" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="K57" t="s">
         <v>206</v>
@@ -48478,33 +48454,33 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="B58" s="3">
-        <v>41162</v>
+        <v>41129</v>
       </c>
       <c r="C58" t="str">
         <f>VLOOKUP(B58,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Legislative scrutiny of budgets</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>218</v>
+        <v>(i) Monitoring of public corporations</v>
+      </c>
+      <c r="D58" t="s">
+        <v>230</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G58" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="K58" t="s">
         <v>206</v>
@@ -48512,17 +48488,17 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="B59" s="3">
-        <v>41129</v>
+        <v>41189</v>
       </c>
       <c r="C59" t="str">
         <f>VLOOKUP(B59,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>(i) Monitoring of public corporations</v>
-      </c>
-      <c r="D59" t="s">
-        <v>230</v>
+        <v>Procurement</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>5</v>
@@ -48531,14 +48507,14 @@
         <v>44</v>
       </c>
       <c r="G59" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="K59" t="s">
         <v>206</v>
@@ -48546,33 +48522,33 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="B60" s="3">
-        <v>41189</v>
+        <v>41127</v>
       </c>
       <c r="C60" t="str">
         <f>VLOOKUP(B60,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Procurement</v>
+        <v>Public access to information</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="G60" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I60" s="1"/>
       <c r="J60" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="K60" t="s">
         <v>206</v>
@@ -48580,33 +48556,33 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B61" s="3">
-        <v>41127</v>
+        <v>41137</v>
       </c>
       <c r="C61" t="str">
         <f>VLOOKUP(B61,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Public access to information</v>
+        <v>Public asset management</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F61" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G61" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I61" s="1"/>
       <c r="J61" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="K61" t="s">
         <v>206</v>
@@ -48614,17 +48590,17 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B62" s="3">
-        <v>41137</v>
+        <v>41167</v>
       </c>
       <c r="C62" t="str">
         <f>VLOOKUP(B62,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Public asset management</v>
+        <v>Revenue administration</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>5</v>
@@ -48633,14 +48609,14 @@
         <v>44</v>
       </c>
       <c r="G62" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="K62" t="s">
         <v>206</v>
@@ -48648,148 +48624,150 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>214</v>
-      </c>
-      <c r="B63" s="3">
-        <v>41167</v>
-      </c>
-      <c r="C63" t="str">
-        <f>VLOOKUP(B63,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Revenue administration</v>
+        <v>71</v>
+      </c>
+      <c r="B63">
+        <v>27470</v>
+      </c>
+      <c r="C63" t="s">
+        <v>357</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>215</v>
+        <v>72</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G63" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I63" s="1"/>
+      <c r="I63" s="1" t="s">
+        <v>382</v>
+      </c>
       <c r="J63" t="s">
-        <v>213</v>
+        <v>70</v>
       </c>
       <c r="K63" t="s">
-        <v>206</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>71</v>
-      </c>
-      <c r="B64">
-        <v>27470</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B64" s="3"/>
       <c r="C64" t="s">
-        <v>363</v>
+        <v>9</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="G64" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>390</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I64" s="1"/>
       <c r="J64" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="K64" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>380</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F65" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G65" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I65" s="1"/>
       <c r="J65" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="K65" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>387</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" t="s">
-        <v>57</v>
+        <v>296</v>
+      </c>
+      <c r="B66" s="3">
+        <v>3326</v>
+      </c>
+      <c r="C66" t="str">
+        <f>VLOOKUP(B66,'[1]Master - API'!$F:$G,2,0)</f>
+        <v>Governance of state-owned enterprises</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>58</v>
+        <v>297</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F66" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G66" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I66" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="J66" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="K66" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>299</v>
-      </c>
-      <c r="B67" s="3">
-        <v>3326</v>
+        <v>40</v>
+      </c>
+      <c r="B67">
+        <v>3310</v>
       </c>
       <c r="C67" t="str">
         <f>VLOOKUP(B67,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Governance of state-owned enterprises</v>
+        <v>Use of command and control regulation</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>300</v>
+        <v>41</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>5</v>
@@ -48798,16 +48776,16 @@
         <v>39</v>
       </c>
       <c r="G67" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J67" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="K67" t="s">
         <v>37</v>
@@ -48815,17 +48793,17 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>40</v>
-      </c>
-      <c r="B68">
-        <v>3310</v>
+        <v>302</v>
+      </c>
+      <c r="B68" s="3">
+        <v>3319</v>
       </c>
       <c r="C68" t="str">
         <f>VLOOKUP(B68,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Use of command and control regulation</v>
+        <v>Direct control over business enterprises</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>41</v>
+        <v>303</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>5</v>
@@ -48834,16 +48812,16 @@
         <v>39</v>
       </c>
       <c r="G68" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J68" t="s">
-        <v>38</v>
+        <v>301</v>
       </c>
       <c r="K68" t="s">
         <v>37</v>
@@ -48851,17 +48829,17 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="B69" s="3">
-        <v>3319</v>
+        <v>3321</v>
       </c>
       <c r="C69" t="str">
         <f>VLOOKUP(B69,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Direct control over business enterprises</v>
+        <v>Government involvement in network sectors</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>5</v>
@@ -48870,16 +48848,16 @@
         <v>39</v>
       </c>
       <c r="G69" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J69" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="K69" t="s">
         <v>37</v>
@@ -48887,17 +48865,17 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B70" s="3">
-        <v>3321</v>
+        <v>3311</v>
       </c>
       <c r="C70" t="str">
         <f>VLOOKUP(B70,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Government involvement in network sectors</v>
+        <v>Price controls</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>5</v>
@@ -48906,16 +48884,16 @@
         <v>39</v>
       </c>
       <c r="G70" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J70" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="K70" t="s">
         <v>37</v>
@@ -48926,11 +48904,11 @@
         <v>308</v>
       </c>
       <c r="B71" s="3">
-        <v>3311</v>
+        <v>3309</v>
       </c>
       <c r="C71" t="str">
         <f>VLOOKUP(B71,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Price controls</v>
+        <v>Scope of state-owned enterprises</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>309</v>
@@ -48942,13 +48920,13 @@
         <v>39</v>
       </c>
       <c r="G71" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J71" t="s">
         <v>307</v>
@@ -48959,35 +48937,35 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>311</v>
+        <v>114</v>
       </c>
       <c r="B72" s="3">
-        <v>3309</v>
+        <v>3305</v>
       </c>
       <c r="C72" t="str">
         <f>VLOOKUP(B72,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Scope of state-owned enterprises</v>
+        <v>Administrative burdens on startups</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>312</v>
+        <v>115</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="G72" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J72" t="s">
-        <v>310</v>
+        <v>113</v>
       </c>
       <c r="K72" t="s">
         <v>37</v>
@@ -48995,17 +48973,17 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>294</v>
       </c>
       <c r="B73" s="3">
-        <v>3305</v>
+        <v>3328</v>
       </c>
       <c r="C73" t="str">
         <f>VLOOKUP(B73,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Administrative burdens on startups</v>
+        <v>Regulatory protection of incumbents</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>115</v>
+        <v>295</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>5</v>
@@ -49014,16 +48992,16 @@
         <v>89</v>
       </c>
       <c r="G73" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J73" t="s">
-        <v>113</v>
+        <v>293</v>
       </c>
       <c r="K73" t="s">
         <v>37</v>
@@ -49031,17 +49009,17 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>297</v>
-      </c>
-      <c r="B74" s="3">
-        <v>3328</v>
+        <v>90</v>
+      </c>
+      <c r="B74">
+        <v>3308</v>
       </c>
       <c r="C74" t="str">
         <f>VLOOKUP(B74,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Regulatory protection of incumbents</v>
+        <v>Other barriers to trade and investment</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>298</v>
+        <v>91</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>5</v>
@@ -49050,16 +49028,16 @@
         <v>89</v>
       </c>
       <c r="G74" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J74" t="s">
-        <v>296</v>
+        <v>88</v>
       </c>
       <c r="K74" t="s">
         <v>37</v>
@@ -49067,17 +49045,17 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B75">
-        <v>3308</v>
+        <v>3307</v>
       </c>
       <c r="C75" t="str">
         <f>VLOOKUP(B75,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Other barriers to trade and investment</v>
+        <v>Explicit barriers to trade and investment</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>5</v>
@@ -49086,16 +49064,16 @@
         <v>89</v>
       </c>
       <c r="G75" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J75" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="K75" t="s">
         <v>37</v>
@@ -49103,17 +49081,17 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B76">
-        <v>3307</v>
+        <v>3323</v>
       </c>
       <c r="C76" t="str">
         <f>VLOOKUP(B76,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Explicit barriers to trade and investment</v>
+        <v>Complexity of regulatory procedures</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>5</v>
@@ -49122,16 +49100,16 @@
         <v>89</v>
       </c>
       <c r="G76" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="J76" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="K76" t="s">
         <v>37</v>
@@ -49139,50 +49117,45 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>108</v>
-      </c>
-      <c r="B77">
-        <v>3323</v>
-      </c>
-      <c r="C77" t="str">
-        <f>VLOOKUP(B77,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Complexity of regulatory procedures</v>
+        <v>187</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" t="s">
+        <v>187</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E77" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E77" t="s">
         <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="G77" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I77" s="1" t="s">
-        <v>392</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I77" s="1"/>
       <c r="J77" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
       <c r="K77" t="s">
-        <v>37</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E78" t="s">
         <v>5</v>
@@ -49191,29 +49164,29 @@
         <v>163</v>
       </c>
       <c r="G78" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I78" s="1"/>
       <c r="J78" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="K78" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E79" t="s">
         <v>5</v>
@@ -49222,14 +49195,14 @@
         <v>163</v>
       </c>
       <c r="G79" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I79" s="1"/>
       <c r="J79" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="K79" t="s">
         <v>161</v>
@@ -49237,14 +49210,14 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E80" t="s">
         <v>5</v>
@@ -49253,14 +49226,14 @@
         <v>163</v>
       </c>
       <c r="G80" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I80" s="1"/>
       <c r="J80" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K80" t="s">
         <v>161</v>
@@ -49268,45 +49241,45 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E81" t="s">
+        <v>160</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F81" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="G81" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I81" s="1"/>
       <c r="J81" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="K81" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>5</v>
@@ -49315,14 +49288,14 @@
         <v>143</v>
       </c>
       <c r="G82" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I82" s="1"/>
       <c r="J82" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K82" t="s">
         <v>141</v>
@@ -49330,14 +49303,14 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>156</v>
+        <v>377</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>5</v>
@@ -49346,14 +49319,14 @@
         <v>143</v>
       </c>
       <c r="G83" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I83" s="1"/>
       <c r="J83" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K83" t="s">
         <v>141</v>
@@ -49361,14 +49334,14 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>383</v>
+        <v>150</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>5</v>
@@ -49377,14 +49350,14 @@
         <v>143</v>
       </c>
       <c r="G84" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I84" s="1"/>
       <c r="J84" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K84" t="s">
         <v>141</v>
@@ -49392,14 +49365,14 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B85" s="3"/>
       <c r="C85" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>5</v>
@@ -49408,14 +49381,14 @@
         <v>143</v>
       </c>
       <c r="G85" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I85" s="1"/>
       <c r="J85" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="K85" t="s">
         <v>141</v>
@@ -49423,297 +49396,294 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>144</v>
-      </c>
-      <c r="B86" s="3"/>
-      <c r="C86" t="s">
-        <v>144</v>
+        <v>201</v>
+      </c>
+      <c r="B86" s="3">
+        <v>41814</v>
+      </c>
+      <c r="C86" t="str">
+        <f>VLOOKUP(B86,'[1]Master - API'!$F:$G,2,0)</f>
+        <v xml:space="preserve">Bureaucratic quality </v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>145</v>
+        <v>202</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F86" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="G86" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I86" s="1"/>
       <c r="J86" t="s">
-        <v>142</v>
-      </c>
-      <c r="K86" t="s">
-        <v>141</v>
+        <v>200</v>
+      </c>
+      <c r="K86" s="6" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>201</v>
+        <v>324</v>
       </c>
       <c r="B87" s="3">
-        <v>41814</v>
+        <v>663</v>
       </c>
       <c r="C87" t="str">
         <f>VLOOKUP(B87,'[1]Master - API'!$F:$G,2,0)</f>
-        <v xml:space="preserve">Bureaucratic quality </v>
+        <v>Diversion of public funds</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>202</v>
+        <v>325</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F87" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="G87" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I87" s="1"/>
       <c r="J87" t="s">
-        <v>200</v>
-      </c>
-      <c r="K87" s="6" t="s">
-        <v>394</v>
+        <v>323</v>
+      </c>
+      <c r="K87" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>330</v>
-      </c>
-      <c r="B88" s="3">
-        <v>663</v>
-      </c>
-      <c r="C88" t="str">
-        <f>VLOOKUP(B88,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Diversion of public funds</v>
+        <v>183</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" t="s">
+        <v>183</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="E88" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E88" t="s">
         <v>5</v>
       </c>
       <c r="F88" t="s">
-        <v>3</v>
+        <v>163</v>
       </c>
       <c r="G88" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I88" s="1"/>
       <c r="J88" t="s">
-        <v>329</v>
+        <v>182</v>
       </c>
       <c r="K88" t="s">
-        <v>328</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>388</v>
+        <v>245</v>
       </c>
       <c r="B89" s="3">
-        <v>32627</v>
+        <v>40985</v>
       </c>
       <c r="C89" t="str">
         <f>VLOOKUP(B89,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>To what extent do you think that corruption is a problem in the public sector in this country? (%)</v>
+        <v>Civil Liberties</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F89" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="G89" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I89" s="1"/>
+      <c r="I89" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="J89" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="K89" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>183</v>
-      </c>
-      <c r="B90" s="3"/>
-      <c r="C90" t="s">
-        <v>183</v>
+        <v>242</v>
+      </c>
+      <c r="B90" s="3">
+        <v>40986</v>
+      </c>
+      <c r="C90" t="str">
+        <f>VLOOKUP(B90,'[1]Master - API'!$F:$G,2,0)</f>
+        <v>Political Rights</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E90" t="s">
+        <v>243</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>163</v>
+        <v>60</v>
       </c>
       <c r="G90" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I90" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>383</v>
+      </c>
       <c r="J90" t="s">
-        <v>182</v>
+        <v>241</v>
       </c>
       <c r="K90" t="s">
-        <v>181</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>245</v>
-      </c>
-      <c r="B91" s="3">
-        <v>40985</v>
-      </c>
-      <c r="C91" t="str">
-        <f>VLOOKUP(B91,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Civil Liberties</v>
+        <v>98</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="C91" t="s">
+        <v>98</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>246</v>
+        <v>99</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F91" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="G91" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>391</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I91" s="1"/>
       <c r="J91" t="s">
-        <v>244</v>
+        <v>97</v>
       </c>
       <c r="K91" t="s">
-        <v>240</v>
+        <v>96</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>242</v>
-      </c>
-      <c r="B92" s="3">
-        <v>40986</v>
-      </c>
-      <c r="C92" t="str">
-        <f>VLOOKUP(B92,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Political Rights</v>
+        <v>176</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" t="s">
+        <v>176</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E92" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E92" t="s">
         <v>5</v>
       </c>
       <c r="F92" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
       <c r="G92" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>391</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="I92" s="1"/>
       <c r="J92" t="s">
-        <v>241</v>
+        <v>175</v>
       </c>
       <c r="K92" t="s">
-        <v>240</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" t="s">
-        <v>98</v>
+        <v>173</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E93" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E93" t="s">
         <v>5</v>
       </c>
       <c r="F93" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="G93" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I93" s="1"/>
       <c r="J93" t="s">
-        <v>97</v>
+        <v>172</v>
       </c>
       <c r="K93" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E94" t="s">
+        <v>130</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F94" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="G94" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I94" s="1"/>
       <c r="J94" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
       <c r="K94" t="s">
         <v>127</v>
@@ -49721,95 +49691,101 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>173</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" t="s">
-        <v>173</v>
+        <v>344</v>
+      </c>
+      <c r="B95" s="3">
+        <v>227</v>
+      </c>
+      <c r="C95" t="str">
+        <f>VLOOKUP(B95,'[1]Master - API'!$F:$G,2,0)</f>
+        <v>Finance / Percent of firms identifying access to finance as a major constraint</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="E95" t="s">
+        <v>345</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F95" t="s">
         <v>163</v>
       </c>
-      <c r="G95" t="s">
-        <v>376</v>
+      <c r="G95" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I95" s="1"/>
       <c r="J95" t="s">
-        <v>172</v>
+        <v>343</v>
       </c>
       <c r="K95" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>129</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" t="s">
-        <v>129</v>
+        <v>333</v>
+      </c>
+      <c r="B96" s="3">
+        <v>308</v>
+      </c>
+      <c r="C96" t="str">
+        <f>VLOOKUP(B96,'[1]Master - API'!$F:$G,2,0)</f>
+        <v>Regulations and Taxes / Percent of firms identifying business licensing and permits as a major constraint</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>130</v>
+        <v>334</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="G96" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I96" s="1"/>
       <c r="J96" t="s">
-        <v>128</v>
+        <v>332</v>
       </c>
       <c r="K96" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>350</v>
+        <v>119</v>
       </c>
       <c r="B97" s="3">
-        <v>227</v>
+        <v>290</v>
       </c>
       <c r="C97" t="str">
         <f>VLOOKUP(B97,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Finance / Percent of firms identifying access to finance as a major constraint</v>
+        <v>Corruption / Percent of firms identifying the courts system as a major constraint</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>351</v>
+        <v>120</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F97" t="s">
-        <v>163</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>376</v>
+        <v>118</v>
+      </c>
+      <c r="G97" t="s">
+        <v>367</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I97" s="1"/>
       <c r="J97" t="s">
-        <v>349</v>
+        <v>117</v>
       </c>
       <c r="K97" t="s">
         <v>116</v>
@@ -49817,17 +49793,17 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="B98" s="3">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="C98" t="str">
         <f>VLOOKUP(B98,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Regulations and Taxes / Percent of firms identifying business licensing and permits as a major constraint</v>
+        <v>Trade / Percent of firms identifying customs and trade regulations as a major constraint</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>5</v>
@@ -49836,14 +49812,14 @@
         <v>89</v>
       </c>
       <c r="G98" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I98" s="1"/>
       <c r="J98" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="K98" t="s">
         <v>116</v>
@@ -49851,33 +49827,33 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>119</v>
+        <v>341</v>
       </c>
       <c r="B99" s="3">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="C99" t="str">
         <f>VLOOKUP(B99,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Corruption / Percent of firms identifying the courts system as a major constraint</v>
+        <v>Workforce / Percent of firms identifying labor regulations as a major constraint</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>120</v>
+        <v>342</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F99" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G99" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I99" s="1"/>
       <c r="J99" t="s">
-        <v>117</v>
+        <v>340</v>
       </c>
       <c r="K99" t="s">
         <v>116</v>
@@ -49885,33 +49861,33 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>336</v>
+        <v>378</v>
       </c>
       <c r="B100" s="3">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="C100" t="str">
         <f>VLOOKUP(B100,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Trade / Percent of firms identifying customs and trade regulations as a major constraint</v>
+        <v>Corruption / Percent of firms identifying corruption as a major constraint</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F100" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="G100" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I100" s="1"/>
       <c r="J100" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="K100" t="s">
         <v>116</v>
@@ -49919,33 +49895,33 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="B101" s="3">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="C101" t="str">
         <f>VLOOKUP(B101,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Workforce / Percent of firms identifying labor regulations as a major constraint</v>
+        <v>Regulations and Taxes / Percent of firms identifying tax administration as a major constraint</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F101" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="G101" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="K101" t="s">
         <v>116</v>
@@ -49953,51 +49929,51 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>384</v>
+        <v>269</v>
       </c>
       <c r="B102" s="3">
-        <v>289</v>
+        <v>28748</v>
       </c>
       <c r="C102" t="str">
         <f>VLOOKUP(B102,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Corruption / Percent of firms identifying corruption as a major constraint</v>
+        <v>Efficient use of assets</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>345</v>
+        <v>270</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F102" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="G102" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I102" s="1"/>
       <c r="J102" t="s">
-        <v>344</v>
+        <v>268</v>
       </c>
       <c r="K102" t="s">
-        <v>116</v>
+        <v>256</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>342</v>
+        <v>266</v>
       </c>
       <c r="B103" s="3">
-        <v>307</v>
+        <v>28749</v>
       </c>
       <c r="C103" t="str">
         <f>VLOOKUP(B103,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Regulations and Taxes / Percent of firms identifying tax administration as a major constraint</v>
+        <v>Environmental policy</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>343</v>
+        <v>267</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>5</v>
@@ -50006,214 +49982,146 @@
         <v>44</v>
       </c>
       <c r="G103" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I103" s="1"/>
       <c r="J103" t="s">
-        <v>341</v>
+        <v>265</v>
       </c>
       <c r="K103" t="s">
-        <v>116</v>
+        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B104" s="3">
-        <v>28748</v>
+        <v>28775</v>
       </c>
       <c r="C104" t="str">
         <f>VLOOKUP(B104,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Efficient use of assets</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>273</v>
+        <v>Separation of powers</v>
+      </c>
+      <c r="D104" t="s">
+        <v>264</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F104" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="G104" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I104" s="1"/>
       <c r="J104" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="K104" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B105" s="3">
-        <v>28749</v>
+        <v>28780</v>
       </c>
       <c r="C105" t="str">
         <f>VLOOKUP(B105,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Environmental policy</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>270</v>
+        <v>State identity</v>
+      </c>
+      <c r="D105" t="s">
+        <v>261</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F105" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="G105" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I105" s="1"/>
       <c r="J105" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="K105" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>266</v>
+        <v>379</v>
       </c>
       <c r="B106" s="3">
-        <v>28775</v>
+        <v>28782</v>
       </c>
       <c r="C106" t="str">
         <f>VLOOKUP(B106,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Separation of powers</v>
-      </c>
-      <c r="D106" t="s">
-        <v>267</v>
+        <v>Steering Capability</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F106" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G106" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I106" s="1"/>
       <c r="J106" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="K106" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>263</v>
-      </c>
-      <c r="B107" s="3">
-        <v>28780</v>
-      </c>
-      <c r="C107" t="str">
-        <f>VLOOKUP(B107,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>State identity</v>
-      </c>
-      <c r="D107" t="s">
-        <v>264</v>
+        <v>375</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F107" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="G107" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" t="s">
-        <v>262</v>
-      </c>
-      <c r="K107" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>385</v>
-      </c>
-      <c r="B108" s="3">
-        <v>28782</v>
-      </c>
-      <c r="C108" t="str">
-        <f>VLOOKUP(B108,'[1]Master - API'!$F:$G,2,0)</f>
-        <v>Steering Capability</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F108" t="s">
-        <v>44</v>
-      </c>
-      <c r="G108" t="s">
-        <v>371</v>
-      </c>
-      <c r="H108" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I108" s="1"/>
-      <c r="J108" t="s">
-        <v>260</v>
-      </c>
-      <c r="K108" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>381</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" t="s">
-        <v>111</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F109" t="s">
-        <v>89</v>
-      </c>
-      <c r="G109" t="s">
-        <v>372</v>
-      </c>
-      <c r="H109" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I109" s="1"/>
-      <c r="J109" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GTMI - Fixed Anti-Corruption to Anticorruption
</commit_message>
<xml_diff>
--- a/data/db_variables.xlsx
+++ b/data/db_variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kannanvenkat/Documents/worldBank/CLAIR/Dashboard/institutional-assessment-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C09CB1-8864-3147-801C-5AC42E8790BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD3272C-0C1E-8441-BE0B-CFEABEE988ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="388">
   <si>
     <t>World Justice Project, Rule of Law</t>
   </si>
@@ -1207,9 +1207,6 @@
     <t>gtmi</t>
   </si>
   <si>
-    <t xml:space="preserve">Anti-corruption, transparency and accountability </t>
-  </si>
-  <si>
     <t>Measures key aspects in the four focus areas of digital transformation in the public sector: core government systems, public service delivery, citizen engagement, and GovTech enablers.</t>
   </si>
   <si>
@@ -46540,8 +46537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C41AAE3-2996-429D-924B-4E57D391677C}">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K107" sqref="K107"/>
+    <sheetView tabSelected="1" topLeftCell="B94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -50120,17 +50117,17 @@
         <v>3</v>
       </c>
       <c r="G107" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>349</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" t="s">
+        <v>386</v>
+      </c>
+      <c r="K107" t="s">
         <v>387</v>
-      </c>
-      <c r="K107" t="s">
-        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin incorporating changes to data ETL
</commit_message>
<xml_diff>
--- a/data/db_variables.xlsx
+++ b/data/db_variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kannanvenkat/Documents/worldBank/CLAIR/Dashboard/institutional-assessment-dashboard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/galileukim_worldbank_org/Documents/github/institutional-assessment-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912D1CDB-C385-754A-9C75-C738BDE09C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{912D1CDB-C385-754A-9C75-C738BDE09C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F04A02CD-03A0-4CE0-9933-0891FEEBD0D3}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{E0EC3B08-D14F-4FE9-A807-BBF74C6FED6F}"/>
   </bookViews>
   <sheets>
     <sheet name="GBID" sheetId="1" r:id="rId1"/>
@@ -46529,29 +46529,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C41AAE3-2996-429D-924B-4E57D391677C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J108" sqref="J108"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" customWidth="1"/>
-    <col min="3" max="3" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.1640625" customWidth="1"/>
-    <col min="11" max="11" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="73.140625" customWidth="1"/>
+    <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>341</v>
       </c>
@@ -46586,7 +46585,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -46620,7 +46619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -46654,7 +46653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>365</v>
       </c>
@@ -46685,7 +46684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -46719,7 +46718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>272</v>
       </c>
@@ -46753,7 +46752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -46784,7 +46783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -46815,7 +46814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -46846,7 +46845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -46877,7 +46876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>275</v>
       </c>
@@ -46911,7 +46910,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>269</v>
       </c>
@@ -46945,7 +46944,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>280</v>
       </c>
@@ -46979,7 +46978,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>278</v>
       </c>
@@ -47013,7 +47012,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>131</v>
       </c>
@@ -47047,7 +47046,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -47078,7 +47077,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>165</v>
       </c>
@@ -47112,7 +47111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>283</v>
       </c>
@@ -47146,7 +47145,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>197</v>
       </c>
@@ -47180,7 +47179,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>247</v>
       </c>
@@ -47214,7 +47213,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>244</v>
       </c>
@@ -47248,7 +47247,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>310</v>
       </c>
@@ -47282,7 +47281,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -47316,7 +47315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>317</v>
       </c>
@@ -47350,7 +47349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>307</v>
       </c>
@@ -47384,7 +47383,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>304</v>
       </c>
@@ -47418,7 +47417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -47452,7 +47451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>241</v>
       </c>
@@ -47486,7 +47485,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>301</v>
       </c>
@@ -47520,7 +47519,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -47554,7 +47553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>134</v>
       </c>
@@ -47588,7 +47587,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>354</v>
       </c>
@@ -47621,7 +47620,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -47652,7 +47651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>100</v>
       </c>
@@ -47683,7 +47682,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>191</v>
       </c>
@@ -47717,7 +47716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>265</v>
       </c>
@@ -47751,7 +47750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>188</v>
       </c>
@@ -47785,7 +47784,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -47816,7 +47815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -47850,7 +47849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -47884,7 +47883,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -47918,7 +47917,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>183</v>
       </c>
@@ -47952,7 +47951,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -47986,7 +47985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>370</v>
       </c>
@@ -48020,7 +48019,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>117</v>
       </c>
@@ -48054,7 +48053,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -48085,7 +48084,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -48116,7 +48115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -48147,7 +48146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -48181,7 +48180,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -48215,7 +48214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>231</v>
       </c>
@@ -48249,7 +48248,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>363</v>
       </c>
@@ -48283,7 +48282,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>216</v>
       </c>
@@ -48317,7 +48316,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>201</v>
       </c>
@@ -48351,7 +48350,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>213</v>
       </c>
@@ -48385,7 +48384,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>210</v>
       </c>
@@ -48419,7 +48418,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -48453,7 +48452,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>204</v>
       </c>
@@ -48487,7 +48486,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>225</v>
       </c>
@@ -48521,7 +48520,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>219</v>
       </c>
@@ -48555,7 +48554,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>207</v>
       </c>
@@ -48589,7 +48588,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -48624,7 +48623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -48655,7 +48654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>369</v>
       </c>
@@ -48686,7 +48685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>288</v>
       </c>
@@ -48722,7 +48721,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -48758,7 +48757,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>293</v>
       </c>
@@ -48794,7 +48793,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>290</v>
       </c>
@@ -48830,7 +48829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>296</v>
       </c>
@@ -48866,7 +48865,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>298</v>
       </c>
@@ -48902,7 +48901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>109</v>
       </c>
@@ -48938,7 +48937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>286</v>
       </c>
@@ -48974,7 +48973,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -49010,7 +49009,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>96</v>
       </c>
@@ -49046,7 +49045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -49082,7 +49081,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>180</v>
       </c>
@@ -49113,7 +49112,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -49144,7 +49143,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>162</v>
       </c>
@@ -49175,7 +49174,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>159</v>
       </c>
@@ -49206,7 +49205,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>154</v>
       </c>
@@ -49237,7 +49236,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>151</v>
       </c>
@@ -49268,7 +49267,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>366</v>
       </c>
@@ -49299,7 +49298,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>145</v>
       </c>
@@ -49330,7 +49329,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>139</v>
       </c>
@@ -49361,7 +49360,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>194</v>
       </c>
@@ -49395,7 +49394,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>314</v>
       </c>
@@ -49429,7 +49428,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>176</v>
       </c>
@@ -49460,7 +49459,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>238</v>
       </c>
@@ -49496,7 +49495,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>235</v>
       </c>
@@ -49532,7 +49531,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -49563,7 +49562,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>171</v>
       </c>
@@ -49594,7 +49593,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>168</v>
       </c>
@@ -49625,7 +49624,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>124</v>
       </c>
@@ -49656,7 +49655,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>334</v>
       </c>
@@ -49690,7 +49689,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>323</v>
       </c>
@@ -49724,7 +49723,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>114</v>
       </c>
@@ -49758,7 +49757,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>320</v>
       </c>
@@ -49792,7 +49791,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>331</v>
       </c>
@@ -49826,7 +49825,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>367</v>
       </c>
@@ -49860,7 +49859,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>326</v>
       </c>
@@ -49894,7 +49893,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>262</v>
       </c>
@@ -49928,7 +49927,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>259</v>
       </c>
@@ -49962,7 +49961,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>256</v>
       </c>
@@ -49996,7 +49995,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>253</v>
       </c>
@@ -50030,7 +50029,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>368</v>
       </c>
@@ -50064,7 +50063,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>364</v>
       </c>
@@ -50094,7 +50093,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>381</v>
       </c>
@@ -50126,13 +50125,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K107" xr:uid="{9C41AAE3-2996-429D-924B-4E57D391677C}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Anticorruption, transparency and accountability"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K107" xr:uid="{9C41AAE3-2996-429D-924B-4E57D391677C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>